<commit_message>
MAT-006: Updated form data reading from Excel file and fixed icon paths
</commit_message>
<xml_diff>
--- a/src/main/resources/02 Teknik listesi.xlsx
+++ b/src/main/resources/02 Teknik listesi.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laptopwork\Doktora\Tez Savunma\Tez İçerik\Model Çalışma\Matriks_Listeler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmetoflu\Desktop\ahmtrdm\material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9532C867-1F92-4D32-8811-8E21D62F6602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4317D9F7-4F99-43C6-B4A3-3B34D987E596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="0" windowWidth="20055" windowHeight="21000" xr2:uid="{0D52DB73-6D49-4C18-8B3C-CA2A4EF74F3F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0D52DB73-6D49-4C18-8B3C-CA2A4EF74F3F}"/>
   </bookViews>
   <sheets>
     <sheet name="İmalat Prosedürleri" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Print_Area" localSheetId="0">'İmalat Prosedürleri'!$I$1:$I$35</definedName>
+    <definedName name="a" localSheetId="0">'İmalat Prosedürleri'!$I$1:$I$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'İmalat Prosedürleri'!$C$1:$J$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -24,12 +24,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="93">
   <si>
     <t>Döküm</t>
   </si>
@@ -292,32 +301,29 @@
     <t>Presleme</t>
   </si>
   <si>
-    <t>Enjeksiyon Kalıp</t>
-  </si>
-  <si>
-    <t>Basınçlı Döküm</t>
-  </si>
-  <si>
-    <t>Katlama Bükme</t>
-  </si>
-  <si>
     <t>Mekanik İşleme NC</t>
   </si>
   <si>
-    <t>Rotasyonel Kalıp</t>
-  </si>
-  <si>
-    <t>Reçine Kalıp</t>
-  </si>
-  <si>
     <t>Termoform</t>
+  </si>
+  <si>
+    <t>Döküm kalıplama</t>
+  </si>
+  <si>
+    <t>Enjeksiyon</t>
+  </si>
+  <si>
+    <t>Reçine Kalıplama</t>
+  </si>
+  <si>
+    <t>Rotasyonel Kalıplama</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,6 +346,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="162"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -434,7 +447,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -735,8 +748,8 @@
   </sheetPr>
   <dimension ref="A1:DR109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +871,12 @@
         <v>29</v>
       </c>
       <c r="F6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="G6" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>0</v>
+      </c>
       <c r="I6" s="8">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -906,7 +924,12 @@
         <v>35</v>
       </c>
       <c r="F8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="G8" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="I8" s="8">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -925,7 +948,12 @@
         <v>36</v>
       </c>
       <c r="F9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="G9" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="I9" s="8">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -953,7 +981,7 @@
         <v>78</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="I10" s="8">
         <f t="shared" si="1"/>
@@ -973,7 +1001,12 @@
         <v>61</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="G11" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="I11" s="8">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -992,7 +1025,12 @@
         <v>55</v>
       </c>
       <c r="F12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="G12" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="I12" s="8">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1011,7 +1049,12 @@
         <v>57</v>
       </c>
       <c r="F13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="G13" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="I13" s="8">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1030,7 +1073,12 @@
         <v>59</v>
       </c>
       <c r="F14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="G14" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="I14" s="8">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1058,7 +1106,7 @@
         <v>79</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I15" s="8">
         <f t="shared" si="1"/>
@@ -1078,7 +1126,12 @@
         <v>40</v>
       </c>
       <c r="F16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="G16" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="I16" s="8">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1097,7 +1150,12 @@
         <v>41</v>
       </c>
       <c r="F17" s="9"/>
-      <c r="H17" s="9"/>
+      <c r="G17" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="I17" s="8">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1125,7 +1183,7 @@
         <v>80</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I18" s="8">
         <f t="shared" si="1"/>
@@ -1145,7 +1203,12 @@
         <v>48</v>
       </c>
       <c r="F19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="G19" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="I19" s="8">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1164,7 +1227,12 @@
         <v>50</v>
       </c>
       <c r="F20" s="9"/>
-      <c r="H20" s="9"/>
+      <c r="G20" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="I20" s="8">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1192,7 +1260,7 @@
         <v>81</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>89</v>
+        <v>12</v>
       </c>
       <c r="I21" s="8">
         <f t="shared" si="1"/>
@@ -1221,7 +1289,7 @@
         <v>82</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I22" s="8">
         <f t="shared" si="1"/>
@@ -1241,7 +1309,12 @@
         <v>15</v>
       </c>
       <c r="F23" s="9"/>
-      <c r="H23" s="9"/>
+      <c r="G23" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>87</v>
+      </c>
       <c r="I23" s="8">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1260,7 +1333,12 @@
         <v>17</v>
       </c>
       <c r="F24" s="9"/>
-      <c r="H24" s="9"/>
+      <c r="G24" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>87</v>
+      </c>
       <c r="I24" s="8">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1279,7 +1357,12 @@
         <v>19</v>
       </c>
       <c r="F25" s="9"/>
-      <c r="H25" s="9"/>
+      <c r="G25" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>87</v>
+      </c>
       <c r="I25" s="8">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1298,7 +1381,12 @@
         <v>21</v>
       </c>
       <c r="F26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="G26" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>87</v>
+      </c>
       <c r="I26" s="8">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1317,7 +1405,12 @@
         <v>23</v>
       </c>
       <c r="F27" s="9"/>
-      <c r="H27" s="9"/>
+      <c r="G27" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>87</v>
+      </c>
       <c r="I27" s="8">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1336,7 +1429,12 @@
         <v>25</v>
       </c>
       <c r="F28" s="9"/>
-      <c r="H28" s="9"/>
+      <c r="G28" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>87</v>
+      </c>
       <c r="I28" s="8">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1364,7 +1462,7 @@
         <v>83</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I29" s="8">
         <f t="shared" si="1"/>
@@ -1393,7 +1491,7 @@
         <v>84</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="I30" s="8">
         <f t="shared" si="1"/>
@@ -1442,7 +1540,12 @@
         <v>67</v>
       </c>
       <c r="F32" s="9"/>
-      <c r="H32" s="9"/>
+      <c r="G32" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="I32" s="8">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -1451,7 +1554,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="3:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C33" s="9"/>
       <c r="D33" s="8">
         <f t="shared" si="0"/>
@@ -1461,7 +1564,12 @@
         <v>69</v>
       </c>
       <c r="F33" s="9"/>
-      <c r="H33" s="9"/>
+      <c r="G33" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="I33" s="8">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -1480,7 +1588,12 @@
         <v>36</v>
       </c>
       <c r="F34" s="9"/>
-      <c r="H34" s="9"/>
+      <c r="G34" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="I34" s="8">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -1499,7 +1612,12 @@
         <v>72</v>
       </c>
       <c r="F35" s="9"/>
-      <c r="H35" s="9"/>
+      <c r="G35" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="I35" s="8">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -1583,6 +1701,7 @@
     <row r="108" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="109" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="85" fitToWidth="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>